<commit_message>
Added colored and black and white plots
</commit_message>
<xml_diff>
--- a/conexoes_corujas.xlsx
+++ b/conexoes_corujas.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlnco\Google Drive\DTI\People analytics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlnco\Google Drive\Udacity\Data Scientist\1st module\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9FCB81-AFBC-4908-99F3-05518F8992BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CF32DB-F115-45F9-9707-B533933C3B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18735" windowHeight="16200" xr2:uid="{0D1AF035-F656-463A-8E06-81B04BA2AB71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,8 +34,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="89">
   <si>
     <t>João Paulo Barbosa Pertence</t>
   </si>
@@ -169,6 +192,138 @@
   </si>
   <si>
     <t>Nome</t>
+  </si>
+  <si>
+    <t>Vera Yasmin Porto</t>
+  </si>
+  <si>
+    <t>Kaique Thiago Thomas Souza</t>
+  </si>
+  <si>
+    <t>Lorena Letícia Viana</t>
+  </si>
+  <si>
+    <t>Tiago Noah Benedito Figueiredo</t>
+  </si>
+  <si>
+    <t>Ruan Emanuel Castro</t>
+  </si>
+  <si>
+    <t>Leandro Iago Diogo Mendes</t>
+  </si>
+  <si>
+    <t>Bryan Luan Peixoto</t>
+  </si>
+  <si>
+    <t>Camila Lúcia Maya das Neves</t>
+  </si>
+  <si>
+    <t>Andrea Valentina Heloisa Pinto</t>
+  </si>
+  <si>
+    <t>Danilo Gustavo Paulo Freitas</t>
+  </si>
+  <si>
+    <t>Vitor Kauê Novaes</t>
+  </si>
+  <si>
+    <t>Pietro Sebastião dos Santos</t>
+  </si>
+  <si>
+    <t>Yuri Sérgio Monteiro</t>
+  </si>
+  <si>
+    <t>Evelyn Liz Alice Campos</t>
+  </si>
+  <si>
+    <t>Otávio Vitor Barros</t>
+  </si>
+  <si>
+    <t>Bernardo Tomás Pietro Porto</t>
+  </si>
+  <si>
+    <t>Mário Rodrigo Nogueira</t>
+  </si>
+  <si>
+    <t>Allana Eloá Rodrigues</t>
+  </si>
+  <si>
+    <t>Silvana Rosa Barbosa</t>
+  </si>
+  <si>
+    <t>Regina Ester Malu Nunes</t>
+  </si>
+  <si>
+    <t>Martin Isaac Ramos</t>
+  </si>
+  <si>
+    <t>Luís João Novaes</t>
+  </si>
+  <si>
+    <t>Francisco Leandro Nathan Fogaça</t>
+  </si>
+  <si>
+    <t>Brenda Josefa Ramos</t>
+  </si>
+  <si>
+    <t>Hugo Miguel Diogo da Cunha</t>
+  </si>
+  <si>
+    <t>Vicente Vitor Heitor Rodrigues</t>
+  </si>
+  <si>
+    <t>Isabela Cláudia Mariane Alves</t>
+  </si>
+  <si>
+    <t>Bryan Breno da Costa</t>
+  </si>
+  <si>
+    <t>Julio Tomás dos Santos</t>
+  </si>
+  <si>
+    <t>Julia Vanessa Gabriela Carvalho</t>
+  </si>
+  <si>
+    <t>Manoel Diego da Cunha</t>
+  </si>
+  <si>
+    <t>Lucca Márcio Viana</t>
+  </si>
+  <si>
+    <t>Ruan Iago Pereira</t>
+  </si>
+  <si>
+    <t>Pedro Francisco Moura</t>
+  </si>
+  <si>
+    <t>Nelson Marcos Vinicius Mateus Almeida</t>
+  </si>
+  <si>
+    <t>Guilherme Leonardo Noah da Rocha</t>
+  </si>
+  <si>
+    <t>Ester Simone Alves</t>
+  </si>
+  <si>
+    <t>Guilherme Luís Renan Figueiredo</t>
+  </si>
+  <si>
+    <t>Cecília Elisa Ana da Paz</t>
+  </si>
+  <si>
+    <t>Enrico Rafael Roberto Aragão</t>
+  </si>
+  <si>
+    <t>Márcia Sabrina Moreira</t>
+  </si>
+  <si>
+    <t>Priscila Gabriela Nicole da Mota</t>
+  </si>
+  <si>
+    <t>Bryan Pietro da Rosa</t>
+  </si>
+  <si>
+    <t>Pietro Thales Jesus</t>
   </si>
 </sst>
 </file>
@@ -523,151 +678,154 @@
   <dimension ref="A1:AS45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="Y1" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="Z1" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="AA1" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="AB1" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="AC1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="AD1" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="AE1" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="AF1" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="AG1" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="AH1" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="AI1" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="AJ1" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="AK1" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="AL1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="AM1" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="AN1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="AO1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="AP1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="AQ1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="AR1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="AS1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -801,7 +959,7 @@
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -935,7 +1093,7 @@
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1069,7 +1227,7 @@
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1203,7 +1361,7 @@
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1337,7 +1495,7 @@
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1471,7 +1629,7 @@
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1605,7 +1763,7 @@
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1739,7 +1897,7 @@
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1873,7 +2031,7 @@
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2007,7 +2165,7 @@
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="B12">
         <v>0.5</v>
@@ -2141,7 +2299,7 @@
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2275,7 +2433,7 @@
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2409,7 +2567,7 @@
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -2543,7 +2701,7 @@
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -2677,7 +2835,7 @@
     </row>
     <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2811,7 +2969,7 @@
     </row>
     <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -2945,7 +3103,7 @@
     </row>
     <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3079,7 +3237,7 @@
     </row>
     <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -3213,7 +3371,7 @@
     </row>
     <row r="21" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3347,7 +3505,7 @@
     </row>
     <row r="22" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -3481,7 +3639,7 @@
     </row>
     <row r="23" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3615,7 +3773,7 @@
     </row>
     <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3749,7 +3907,7 @@
     </row>
     <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3883,7 +4041,7 @@
     </row>
     <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4017,7 +4175,7 @@
     </row>
     <row r="27" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -4151,7 +4309,7 @@
     </row>
     <row r="28" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4285,7 +4443,7 @@
     </row>
     <row r="29" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -4419,7 +4577,7 @@
     </row>
     <row r="30" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -4553,7 +4711,7 @@
     </row>
     <row r="31" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="B31">
         <v>0.5</v>
@@ -4687,7 +4845,7 @@
     </row>
     <row r="32" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -4821,7 +4979,7 @@
     </row>
     <row r="33" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B33">
         <v>0.5</v>
@@ -4955,7 +5113,7 @@
     </row>
     <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -5089,7 +5247,7 @@
     </row>
     <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5223,7 +5381,7 @@
     </row>
     <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -5357,7 +5515,7 @@
     </row>
     <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -5491,7 +5649,7 @@
     </row>
     <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B38">
         <v>0.5</v>
@@ -5625,7 +5783,7 @@
     </row>
     <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="B39">
         <v>0.5</v>
@@ -5759,7 +5917,7 @@
     </row>
     <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -5893,7 +6051,7 @@
     </row>
     <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -6027,7 +6185,7 @@
     </row>
     <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -6161,7 +6319,7 @@
     </row>
     <row r="43" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B43">
         <v>0.5</v>
@@ -6295,7 +6453,7 @@
     </row>
     <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B44">
         <v>0.5</v>
@@ -6429,7 +6587,7 @@
     </row>
     <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B45">
         <v>0.5</v>
@@ -6564,4 +6722,511 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CE7B73-CE94-4E5D-8198-C82EDE193952}">
+  <dimension ref="A1:AV44"/>
+  <sheetViews>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:AV1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="str" cm="1">
+        <f t="array" ref="E1:AV1">TRANSPOSE(B1:B44)</f>
+        <v>Allana Eloá Rodrigues</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Andrea Valentina Heloisa Pinto</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Bernardo Tomás Pietro Porto</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Brenda Josefa Ramos</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Bryan Breno da Costa</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Bryan Luan Peixoto</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Bryan Pietro da Rosa</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Camila Lúcia Maya das Neves</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Cecília Elisa Ana da Paz</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Danilo Gustavo Paulo Freitas</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Enrico Rafael Roberto Aragão</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Ester Simone Alves</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>Evelyn Liz Alice Campos</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Francisco Leandro Nathan Fogaça</v>
+      </c>
+      <c r="S1" t="str">
+        <v>Guilherme Leonardo Noah da Rocha</v>
+      </c>
+      <c r="T1" t="str">
+        <v>Guilherme Luís Renan Figueiredo</v>
+      </c>
+      <c r="U1" t="str">
+        <v>Hugo Miguel Diogo da Cunha</v>
+      </c>
+      <c r="V1" t="str">
+        <v>Isabela Cláudia Mariane Alves</v>
+      </c>
+      <c r="W1" t="str">
+        <v>Julia Vanessa Gabriela Carvalho</v>
+      </c>
+      <c r="X1" t="str">
+        <v>Julio Tomás dos Santos</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>Kaique Thiago Thomas Souza</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>Leandro Iago Diogo Mendes</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>Lorena Letícia Viana</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>Lucca Márcio Viana</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>Luís João Novaes</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>Manoel Diego da Cunha</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>Márcia Sabrina Moreira</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>Mário Rodrigo Nogueira</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>Martin Isaac Ramos</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>Nelson Marcos Vinicius Mateus Almeida</v>
+      </c>
+      <c r="AI1" t="str">
+        <v>Otávio Vitor Barros</v>
+      </c>
+      <c r="AJ1" t="str">
+        <v>Pedro Francisco Moura</v>
+      </c>
+      <c r="AK1" t="str">
+        <v>Pietro Sebastião dos Santos</v>
+      </c>
+      <c r="AL1" t="str">
+        <v>Pietro Thales Jesus</v>
+      </c>
+      <c r="AM1" t="str">
+        <v>Priscila Gabriela Nicole da Mota</v>
+      </c>
+      <c r="AN1" t="str">
+        <v>Regina Ester Malu Nunes</v>
+      </c>
+      <c r="AO1" t="str">
+        <v>Ruan Emanuel Castro</v>
+      </c>
+      <c r="AP1" t="str">
+        <v>Ruan Iago Pereira</v>
+      </c>
+      <c r="AQ1" t="str">
+        <v>Silvana Rosa Barbosa</v>
+      </c>
+      <c r="AR1" t="str">
+        <v>Tiago Noah Benedito Figueiredo</v>
+      </c>
+      <c r="AS1" t="str">
+        <v>Vera Yasmin Porto</v>
+      </c>
+      <c r="AT1" t="str">
+        <v>Vicente Vitor Heitor Rodrigues</v>
+      </c>
+      <c r="AU1" t="str">
+        <v>Vitor Kauê Novaes</v>
+      </c>
+      <c r="AV1" t="str">
+        <v>Yuri Sérgio Monteiro</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B44">
+    <sortCondition ref="B1:B44"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>